<commit_message>
Sites.cs;  money -> oil; material -> metal
</commit_message>
<xml_diff>
--- a/BuildingsConfiguration.xlsx
+++ b/BuildingsConfiguration.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Food Family</t>
   </si>
@@ -119,7 +119,13 @@
     <t>PopUp/2 Min</t>
   </si>
   <si>
-    <t>DryUpTime (Sec)</t>
+    <t>DryUpTime (Sec) ?</t>
+  </si>
+  <si>
+    <t>Turret Family</t>
+  </si>
+  <si>
+    <t>Health</t>
   </si>
 </sst>
 </file>
@@ -175,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -198,11 +204,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -219,9 +247,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -229,6 +254,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -511,50 +554,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="N20" sqref="N20:P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" style="1" customWidth="1"/>
-    <col min="2" max="4" width="11.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="5" customWidth="1"/>
-    <col min="6" max="8" width="11.28515625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="5" customWidth="1"/>
-    <col min="10" max="12" width="11.28515625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" style="5" customWidth="1"/>
-    <col min="14" max="16" width="11.28515625" style="7" customWidth="1"/>
+    <col min="2" max="4" width="11.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="2.42578125" style="5" customWidth="1"/>
+    <col min="6" max="8" width="11.28515625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="2" style="5" customWidth="1"/>
+    <col min="10" max="12" width="11.28515625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="2.5703125" style="5" customWidth="1"/>
+    <col min="14" max="16" width="11.28515625" style="6" customWidth="1"/>
+    <col min="17" max="17" width="2.5703125" style="12" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" style="11" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" style="11" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" style="17" customWidth="1"/>
+    <col min="21" max="22" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="J1" s="6" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="J1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="N1" s="6" t="s">
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="N1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="R1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+    </row>
+    <row r="2" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -594,8 +652,13 @@
       <c r="P2" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -611,154 +674,159 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="F4" s="7">
-        <v>300</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="F4" s="6">
+        <v>300</v>
+      </c>
+      <c r="G4" s="6">
         <v>400</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>600</v>
       </c>
-      <c r="J4" s="7">
-        <v>300</v>
-      </c>
-      <c r="K4" s="7">
+      <c r="J4" s="6">
+        <v>300</v>
+      </c>
+      <c r="K4" s="6">
         <v>400</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="6">
         <v>600</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="6">
         <v>400</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="6">
         <v>800</v>
       </c>
-      <c r="P4" s="9">
+      <c r="P4" s="8">
         <v>1600</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7">
-        <v>300</v>
-      </c>
-      <c r="C5" s="7">
+      <c r="B5" s="6">
+        <v>300</v>
+      </c>
+      <c r="C5" s="6">
         <v>600</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>1000</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="J5" s="7">
-        <v>300</v>
-      </c>
-      <c r="K5" s="7">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="J5" s="6">
+        <v>300</v>
+      </c>
+      <c r="K5" s="6">
         <v>600</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="8">
         <v>1000</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="6">
         <v>400</v>
       </c>
-      <c r="O5" s="7">
+      <c r="O5" s="6">
         <v>800</v>
       </c>
-      <c r="P5" s="9">
+      <c r="P5" s="8">
         <v>1600</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7">
-        <v>300</v>
-      </c>
-      <c r="C6" s="7">
+      <c r="B6" s="6">
+        <v>300</v>
+      </c>
+      <c r="C6" s="6">
         <v>400</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>600</v>
       </c>
-      <c r="F6" s="7">
-        <v>300</v>
-      </c>
-      <c r="G6" s="7">
+      <c r="F6" s="6">
+        <v>300</v>
+      </c>
+      <c r="G6" s="6">
         <v>600</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>1000</v>
       </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="N6" s="7">
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="N6" s="6">
         <v>400</v>
       </c>
-      <c r="O6" s="7">
+      <c r="O6" s="6">
         <v>800</v>
       </c>
-      <c r="P6" s="9">
+      <c r="P6" s="8">
         <v>1600</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>4</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>2</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>10</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>4</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>6</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>8</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <v>3</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <v>6</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="6">
         <v>10</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="6">
         <v>-2</v>
       </c>
-      <c r="O7" s="7">
+      <c r="O7" s="6">
         <v>-5</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7" s="6">
         <v>-15</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -773,101 +841,101 @@
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>10</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>20</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>40</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="F10" s="7">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="F10" s="6">
         <v>10</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>20</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>40</v>
       </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="7">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="6">
         <v>3</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="6">
         <v>10</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <v>20</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="6">
         <v>40</v>
       </c>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="6">
         <v>1</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="7">
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="6">
         <v>1</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -882,106 +950,106 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="F14" s="7">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="F14" s="6">
         <v>4</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="6">
         <v>6</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="6">
         <v>10</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="6">
         <v>2</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="6">
         <v>4</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="6">
         <v>8</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N14" s="6">
         <v>2</v>
       </c>
-      <c r="O14" s="7">
+      <c r="O14" s="6">
         <v>4</v>
       </c>
-      <c r="P14" s="7">
+      <c r="P14" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>2</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>3</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>4</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="J15" s="7">
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="J15" s="6">
         <v>4</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="6">
         <v>6</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="6">
         <v>10</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15" s="6">
         <v>2</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O15" s="6">
         <v>4</v>
       </c>
-      <c r="P15" s="7">
+      <c r="P15" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>3</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>5</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>1</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>2</v>
       </c>
-      <c r="H16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="N16" s="7">
+      <c r="H16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="N16" s="6">
         <v>2</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O16" s="6">
         <v>4</v>
       </c>
-      <c r="P16" s="7">
+      <c r="P16" s="6">
         <v>8</v>
       </c>
     </row>
@@ -989,32 +1057,32 @@
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="7">
+      <c r="C17" s="7"/>
+      <c r="D17" s="6">
         <v>1</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>1</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>1</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="6">
         <v>2</v>
       </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="7">
+      <c r="J17" s="7"/>
+      <c r="K17" s="6">
         <v>1</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L17" s="6">
         <v>2</v>
       </c>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
@@ -1035,58 +1103,85 @@
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>420</v>
       </c>
-      <c r="C19" s="7">
-        <v>300</v>
-      </c>
-      <c r="D19" s="7">
+      <c r="C19" s="6">
+        <v>300</v>
+      </c>
+      <c r="D19" s="6">
         <v>600</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>420</v>
       </c>
-      <c r="G19" s="7">
-        <v>300</v>
-      </c>
-      <c r="H19" s="7">
+      <c r="G19" s="6">
+        <v>300</v>
+      </c>
+      <c r="H19" s="6">
         <v>600</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="6">
         <v>420</v>
       </c>
-      <c r="K19" s="7">
-        <v>300</v>
-      </c>
-      <c r="L19" s="7">
+      <c r="K19" s="6">
+        <v>300</v>
+      </c>
+      <c r="L19" s="6">
         <v>600</v>
       </c>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
+      <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="18">
+        <v>150</v>
+      </c>
+      <c r="C20" s="18">
+        <v>300</v>
+      </c>
+      <c r="D20" s="18">
+        <v>500</v>
+      </c>
+      <c r="F20" s="18">
+        <v>150</v>
+      </c>
+      <c r="G20" s="18">
+        <v>300</v>
+      </c>
+      <c r="H20" s="18">
+        <v>500</v>
+      </c>
+      <c r="J20" s="18">
+        <v>150</v>
+      </c>
+      <c r="K20" s="18">
+        <v>300</v>
+      </c>
+      <c r="L20" s="18">
+        <v>500</v>
+      </c>
+      <c r="N20" s="18">
+        <v>150</v>
+      </c>
+      <c r="O20" s="18">
+        <v>300</v>
+      </c>
+      <c r="P20" s="18">
+        <v>500</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="N1:P1"/>
+    <mergeCell ref="R1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>